<commit_message>
Fill in model selection values
</commit_message>
<xml_diff>
--- a/results/hindcast_output/model_selection.xlsx
+++ b/results/hindcast_output/model_selection.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\howar\Documents\Oregon State\ELH_WestCoast\results\hindcast_output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FA10AAF-944F-4FAC-8BB0-4FB1EC8862C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BCB289D-2DB6-4D8C-93C3-27F42CEC9DEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="41">
   <si>
     <t>Species</t>
   </si>
@@ -68,18 +68,9 @@
     <t>u_vint_50m: u-eastward vertically integrated from 0-50m and averaged from coast to 50 km offshore</t>
   </si>
   <si>
-    <t>u 100m vertically integrated</t>
-  </si>
-  <si>
-    <t>u 50m vertically integrated</t>
-  </si>
-  <si>
     <t>spice</t>
   </si>
   <si>
-    <t>CA undercurrent</t>
-  </si>
-  <si>
     <t>vmax_cu</t>
   </si>
   <si>
@@ -117,13 +108,58 @@
   </si>
   <si>
     <t>Log-likelihood</t>
+  </si>
+  <si>
+    <t>iso26</t>
+  </si>
+  <si>
+    <t>vgeo: surface geostrophic v-component avg from coast to 50km</t>
+  </si>
+  <si>
+    <t>iso26: depth of the 26 isopycnal</t>
+  </si>
+  <si>
+    <t>vmax_cu: max v at core of CA undercurrent</t>
+  </si>
+  <si>
+    <t>Northern Anchovy</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Upwelling appears to be more important to smaller sizes/earlier life stages</t>
+  </si>
+  <si>
+    <t>Water masses appear to be more important to larger sizes/later life stages</t>
+  </si>
+  <si>
+    <t>CA undercurrent important to early stages of sanddab and later stages of anchovy</t>
+  </si>
+  <si>
+    <t>Geostrophic surface transport important to early stages of hake and later stages of shortbelly</t>
+  </si>
+  <si>
+    <t>Pacific Sanddab</t>
+  </si>
+  <si>
+    <t>Shortbelly Rockfish</t>
+  </si>
+  <si>
+    <t>Widow Rockfish</t>
+  </si>
+  <si>
+    <t>Market Squid</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -147,8 +183,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -158,6 +211,30 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -174,15 +251,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -190,6 +264,21 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -470,10 +559,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A1:A7"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -498,11 +587,11 @@
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" t="s">
-        <v>15</v>
+      <c r="B2" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>27</v>
       </c>
       <c r="E2" t="s">
         <v>9</v>
@@ -512,11 +601,11 @@
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" t="s">
-        <v>16</v>
+      <c r="B3" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>14</v>
       </c>
       <c r="E3" t="s">
         <v>10</v>
@@ -526,11 +615,11 @@
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="7" t="s">
         <v>13</v>
-      </c>
-      <c r="C4" t="s">
-        <v>14</v>
       </c>
       <c r="E4" t="s">
         <v>11</v>
@@ -540,11 +629,11 @@
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" t="s">
-        <v>15</v>
+      <c r="B5" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="E5" t="s">
         <v>12</v>
@@ -554,19 +643,58 @@
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C6" t="s">
-        <v>18</v>
+      <c r="B6" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="B7" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="7" t="s">
         <v>13</v>
+      </c>
+      <c r="E7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -576,10 +704,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{494A45B2-305D-490A-9F7F-E122BE2F71EC}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="H80" sqref="H80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -591,13 +719,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>19</v>
+      <c r="A1" s="12" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>1</v>
@@ -610,55 +738,55 @@
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
       <c r="B4" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B5" s="4">
         <v>-7648</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="4">
         <v>64.8</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="4">
         <v>-5008</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="4">
         <v>76.900000000000006</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="6">
+        <v>18</v>
+      </c>
+      <c r="B6" s="5">
         <v>-7622</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="5">
         <v>64.92</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="4">
         <v>-5001</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="4">
         <v>76.900000000000006</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B7" s="4">
         <v>-7652</v>
@@ -666,16 +794,16 @@
       <c r="C7" s="4">
         <v>64.78</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="4">
         <v>-5010</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="4">
         <v>76.900000000000006</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B8" s="4">
         <v>-7632</v>
@@ -683,16 +811,16 @@
       <c r="C8" s="4">
         <v>64.87</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="4">
         <v>-5010</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="4">
         <v>76.900000000000006</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B9" s="4">
         <v>-7634</v>
@@ -700,33 +828,33 @@
       <c r="C9" s="4">
         <v>64.87</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="4">
         <v>-5011</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="4">
         <v>76.900000000000006</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D10" s="6">
+        <v>24</v>
+      </c>
+      <c r="D10" s="5">
         <v>-4963</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E10" s="5">
         <v>77.099999999999994</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B11" s="4">
         <v>-7626</v>
@@ -737,25 +865,787 @@
       <c r="D11" s="3">
         <v>-4992</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11" s="4">
         <v>77</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="4">
+        <v>-5022</v>
+      </c>
+      <c r="E12" s="4">
+        <v>76.8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" s="12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" s="1"/>
+      <c r="B18" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D12" s="5">
-        <v>-5022</v>
-      </c>
-      <c r="E12" s="5">
-        <v>76.8</v>
+      <c r="D18" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" s="11">
+        <v>-1413</v>
+      </c>
+      <c r="E19" s="11">
+        <v>74.3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" s="11">
+        <v>-1055</v>
+      </c>
+      <c r="C20" s="11">
+        <v>78</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D21" s="3">
+        <v>-1429</v>
+      </c>
+      <c r="E21" s="3">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A22" s="2"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A24" s="12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A26" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A27" s="1"/>
+      <c r="B27" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A28" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B28" s="11">
+        <v>-1167</v>
+      </c>
+      <c r="C28" s="11">
+        <v>71.900000000000006</v>
+      </c>
+      <c r="D28" s="4">
+        <v>-2743</v>
+      </c>
+      <c r="E28" s="4">
+        <v>48.1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A29" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B29" s="3">
+        <v>-1171</v>
+      </c>
+      <c r="C29" s="3">
+        <v>71.8</v>
+      </c>
+      <c r="D29" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="E29" s="13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A30" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D30" s="13">
+        <v>-2740</v>
+      </c>
+      <c r="E30" s="13">
+        <v>48.1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A31" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D31" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="E31" s="13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A32" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D32" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="E32" s="13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A33" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B33" s="3">
+        <v>-1173</v>
+      </c>
+      <c r="C33" s="3">
+        <v>71.8</v>
+      </c>
+      <c r="D33" s="13">
+        <v>-2770</v>
+      </c>
+      <c r="E33" s="13">
+        <v>47.5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A34" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B34" s="3">
+        <v>-1167</v>
+      </c>
+      <c r="C34" s="3">
+        <v>71.900000000000006</v>
+      </c>
+      <c r="D34" s="5">
+        <v>-2694</v>
+      </c>
+      <c r="E34" s="5">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A35" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B35" s="4">
+        <v>-1184</v>
+      </c>
+      <c r="C35" s="4">
+        <v>71.5</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A38" s="12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A40" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A41" s="1"/>
+      <c r="B41" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A42" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B42">
+        <v>-5955</v>
+      </c>
+      <c r="C42" s="14">
+        <v>70.900000000000006</v>
+      </c>
+      <c r="D42">
+        <v>-4383</v>
+      </c>
+      <c r="E42">
+        <v>78.900000000000006</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A43" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B43">
+        <v>-5940</v>
+      </c>
+      <c r="C43" s="14">
+        <v>71</v>
+      </c>
+      <c r="D43" s="6">
+        <v>-4308</v>
+      </c>
+      <c r="E43" s="6">
+        <v>79.2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A44" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B44">
+        <v>-5954</v>
+      </c>
+      <c r="C44" s="14">
+        <v>70.900000000000006</v>
+      </c>
+      <c r="D44">
+        <v>-4382</v>
+      </c>
+      <c r="E44">
+        <v>78.900000000000006</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A45" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B45">
+        <v>-5934</v>
+      </c>
+      <c r="C45" s="14">
+        <v>71</v>
+      </c>
+      <c r="D45">
+        <v>-4337</v>
+      </c>
+      <c r="E45">
+        <v>79.099999999999994</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A46" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B46">
+        <v>-5930</v>
+      </c>
+      <c r="C46" s="14">
+        <v>71</v>
+      </c>
+      <c r="D46">
+        <v>-4343</v>
+      </c>
+      <c r="E46">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A47" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B47" s="6">
+        <v>-5905</v>
+      </c>
+      <c r="C47" s="15">
+        <v>71.2</v>
+      </c>
+      <c r="D47">
+        <v>-4355</v>
+      </c>
+      <c r="E47">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A48" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B48">
+        <v>-5920</v>
+      </c>
+      <c r="C48" s="14">
+        <v>71.099999999999994</v>
+      </c>
+      <c r="D48">
+        <v>-4387</v>
+      </c>
+      <c r="E48">
+        <v>78.900000000000006</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A49" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B49">
+        <v>-5983</v>
+      </c>
+      <c r="C49" s="14">
+        <v>70.8</v>
+      </c>
+      <c r="D49">
+        <v>-4392</v>
+      </c>
+      <c r="E49">
+        <v>78.900000000000006</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A52" s="16" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A54" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C54" s="1"/>
+      <c r="D54" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A55" s="1"/>
+      <c r="B55" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A56" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B56">
+        <v>-1643</v>
+      </c>
+      <c r="C56">
+        <v>89.7</v>
+      </c>
+      <c r="D56">
+        <v>-3053</v>
+      </c>
+      <c r="E56">
+        <v>84.3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A57" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B57">
+        <v>-1640</v>
+      </c>
+      <c r="C57">
+        <v>89.7</v>
+      </c>
+      <c r="D57">
+        <v>-3045</v>
+      </c>
+      <c r="E57">
+        <v>84.3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A58" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B58">
+        <v>-1642</v>
+      </c>
+      <c r="C58">
+        <v>89.7</v>
+      </c>
+      <c r="D58">
+        <v>-3052</v>
+      </c>
+      <c r="E58">
+        <v>84.3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A59" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B59">
+        <v>-1643.3</v>
+      </c>
+      <c r="C59">
+        <v>89.7</v>
+      </c>
+      <c r="D59">
+        <v>-3059</v>
+      </c>
+      <c r="E59">
+        <v>84.2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A60" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B60">
+        <v>-1642</v>
+      </c>
+      <c r="C60">
+        <v>89.7</v>
+      </c>
+      <c r="D60">
+        <v>-3060</v>
+      </c>
+      <c r="E60">
+        <v>84.2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A61" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B61" s="6">
+        <v>-1639</v>
+      </c>
+      <c r="C61" s="6">
+        <v>89.7</v>
+      </c>
+      <c r="D61">
+        <v>-3022</v>
+      </c>
+      <c r="E61">
+        <v>84.4</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A62" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B62">
+        <v>-1651</v>
+      </c>
+      <c r="C62">
+        <v>89.6</v>
+      </c>
+      <c r="D62" s="6">
+        <v>-3018</v>
+      </c>
+      <c r="E62" s="6">
+        <v>84.4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A63" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B63">
+        <v>-1642</v>
+      </c>
+      <c r="C63">
+        <v>89.7</v>
+      </c>
+      <c r="D63">
+        <v>-3071</v>
+      </c>
+      <c r="E63">
+        <v>84.2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A66" s="12" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A68" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C68" s="1"/>
+      <c r="D68" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A69" s="1"/>
+      <c r="B69" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A70" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B70">
+        <v>-4214</v>
+      </c>
+      <c r="C70">
+        <v>75.5</v>
+      </c>
+      <c r="D70">
+        <v>-2084</v>
+      </c>
+      <c r="E70">
+        <v>84.7</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A71" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B71">
+        <v>-4205</v>
+      </c>
+      <c r="C71">
+        <v>75.5</v>
+      </c>
+      <c r="D71">
+        <v>-2084</v>
+      </c>
+      <c r="E71">
+        <v>84.7</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A72" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B72">
+        <v>-4211</v>
+      </c>
+      <c r="C72">
+        <v>75.5</v>
+      </c>
+      <c r="D72">
+        <v>-2084</v>
+      </c>
+      <c r="E72">
+        <v>84.7</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A73" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B73">
+        <v>-4221</v>
+      </c>
+      <c r="C73">
+        <v>75.400000000000006</v>
+      </c>
+      <c r="D73">
+        <v>-2080</v>
+      </c>
+      <c r="E73">
+        <v>84.7</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A74" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B74">
+        <v>-4226</v>
+      </c>
+      <c r="C74">
+        <v>75.400000000000006</v>
+      </c>
+      <c r="D74">
+        <v>-2079</v>
+      </c>
+      <c r="E74">
+        <v>84.8</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A75" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B75" s="6">
+        <v>-4203</v>
+      </c>
+      <c r="C75" s="6">
+        <v>75.5</v>
+      </c>
+      <c r="D75">
+        <v>-2068</v>
+      </c>
+      <c r="E75">
+        <v>84.8</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A76" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B76">
+        <v>-4234</v>
+      </c>
+      <c r="C76">
+        <v>75.3</v>
+      </c>
+      <c r="D76" s="6">
+        <v>-2065</v>
+      </c>
+      <c r="E76" s="6">
+        <v>84.9</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A77" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B77">
+        <v>-4252</v>
+      </c>
+      <c r="C77">
+        <v>75.2</v>
+      </c>
+      <c r="D77">
+        <v>-2084</v>
+      </c>
+      <c r="E77">
+        <v>84.7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add rescaled predictions, update anchovy and sanddab models
</commit_message>
<xml_diff>
--- a/results/hindcast_output/model_selection.xlsx
+++ b/results/hindcast_output/model_selection.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\howar\Documents\Oregon State\ELH_WestCoast\results\hindcast_output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BCB289D-2DB6-4D8C-93C3-27F42CEC9DEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52B3CF6A-2D10-40C6-92CB-2022C179BCD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Models" sheetId="1" r:id="rId1"/>
     <sheet name="Statistics" sheetId="2" r:id="rId2"/>
-    <sheet name="Cross Validation" sheetId="3" r:id="rId3"/>
+    <sheet name="Schoener's D" sheetId="4" r:id="rId3"/>
+    <sheet name="Cross Validation" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="44">
   <si>
     <t>Species</t>
   </si>
@@ -150,6 +151,15 @@
   </si>
   <si>
     <t>Market Squid</t>
+  </si>
+  <si>
+    <t>uvint 100m</t>
+  </si>
+  <si>
+    <t>uvint 50m</t>
+  </si>
+  <si>
+    <t>Schoener's D</t>
   </si>
 </sst>
 </file>
@@ -228,13 +238,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
+        <fgColor theme="3" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.79998168889431442"/>
+        <fgColor rgb="FFF1E0F4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -251,7 +261,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -268,23 +278,43 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFF1E0F4"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -561,8 +591,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -601,11 +631,11 @@
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>14</v>
+      <c r="B3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>41</v>
       </c>
       <c r="E3" t="s">
         <v>10</v>
@@ -615,11 +645,11 @@
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>13</v>
+      <c r="B4" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>41</v>
       </c>
       <c r="E4" t="s">
         <v>11</v>
@@ -704,10 +734,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{494A45B2-305D-490A-9F7F-E122BE2F71EC}">
-  <dimension ref="A1:E77"/>
+  <dimension ref="A1:E82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
-      <selection activeCell="H80" sqref="H80"/>
+    <sheetView topLeftCell="A66" workbookViewId="0">
+      <selection activeCell="I41" sqref="I41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -719,7 +749,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="11" t="s">
         <v>16</v>
       </c>
     </row>
@@ -887,7 +917,7 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" s="12" t="s">
+      <c r="A15" s="11" t="s">
         <v>31</v>
       </c>
     </row>
@@ -920,7 +950,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>24</v>
@@ -928,544 +958,544 @@
       <c r="C19" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D19" s="11">
-        <v>-1413</v>
-      </c>
-      <c r="E19" s="11">
-        <v>74.3</v>
+      <c r="D19" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="E19" s="16" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B20" s="11">
-        <v>-1055</v>
-      </c>
-      <c r="C20" s="11">
-        <v>78</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>24</v>
+        <v>18</v>
+      </c>
+      <c r="B20" s="10">
+        <v>-978</v>
+      </c>
+      <c r="C20" s="10">
+        <v>74.5</v>
+      </c>
+      <c r="D20" s="3">
+        <v>-1416</v>
+      </c>
+      <c r="E20" s="3">
+        <v>67.599999999999994</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A22" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" s="3">
+        <v>-979</v>
+      </c>
+      <c r="C22" s="3">
+        <v>74.400000000000006</v>
+      </c>
+      <c r="D22" s="3">
+        <v>-1409</v>
+      </c>
+      <c r="E22" s="3">
+        <v>67.8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A23" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" s="3">
+        <v>-980</v>
+      </c>
+      <c r="C23" s="3">
+        <v>74.400000000000006</v>
+      </c>
+      <c r="D23" s="10">
+        <v>-1407</v>
+      </c>
+      <c r="E23" s="10">
+        <v>67.8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A24" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B24" s="3">
+        <v>-985</v>
+      </c>
+      <c r="C24" s="3">
+        <v>74.3</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A25" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D21" s="3">
-        <v>-1429</v>
-      </c>
-      <c r="E21" s="3">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A22" s="2"/>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A24" s="12" t="s">
+      <c r="B25" s="3">
+        <v>-981</v>
+      </c>
+      <c r="C25" s="3">
+        <v>74.400000000000006</v>
+      </c>
+      <c r="D25" s="3">
+        <v>-1416</v>
+      </c>
+      <c r="E25" s="3">
+        <v>67.599999999999994</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B26" s="3">
+        <v>-985</v>
+      </c>
+      <c r="C26" s="3">
+        <v>74.3</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A27" s="2"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A29" s="11" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A26" s="1" t="s">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A31" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B31" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1" t="s">
+      <c r="C31" s="1"/>
+      <c r="D31" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A27" s="1"/>
-      <c r="B27" s="2" t="s">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A32" s="1"/>
+      <c r="B32" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C32" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="D32" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E27" s="2" t="s">
+      <c r="E32" s="2" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A28" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B28" s="11">
-        <v>-1167</v>
-      </c>
-      <c r="C28" s="11">
-        <v>71.900000000000006</v>
-      </c>
-      <c r="D28" s="4">
-        <v>-2743</v>
-      </c>
-      <c r="E28" s="4">
-        <v>48.1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A29" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B29" s="3">
-        <v>-1171</v>
-      </c>
-      <c r="C29" s="3">
-        <v>71.8</v>
-      </c>
-      <c r="D29" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="E29" s="13" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A30" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D30" s="13">
-        <v>-2740</v>
-      </c>
-      <c r="E30" s="13">
-        <v>48.1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A31" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D31" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="E31" s="13" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A32" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D32" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="E32" s="13" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B33" s="3">
-        <v>-1173</v>
-      </c>
-      <c r="C33" s="3">
-        <v>71.8</v>
-      </c>
-      <c r="D33" s="13">
-        <v>-2770</v>
-      </c>
-      <c r="E33" s="13">
-        <v>47.5</v>
+        <v>17</v>
+      </c>
+      <c r="B33" s="16">
+        <v>-796</v>
+      </c>
+      <c r="C33" s="18">
+        <v>74.8</v>
+      </c>
+      <c r="D33" s="4">
+        <v>-2028</v>
+      </c>
+      <c r="E33" s="4">
+        <v>48.9</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B34" s="3">
-        <v>-1167</v>
-      </c>
-      <c r="C34" s="3">
-        <v>71.900000000000006</v>
-      </c>
-      <c r="D34" s="5">
-        <v>-2694</v>
-      </c>
-      <c r="E34" s="5">
-        <v>49</v>
+        <v>-780</v>
+      </c>
+      <c r="C34" s="19">
+        <v>74.8</v>
+      </c>
+      <c r="D34" s="4">
+        <v>-2037</v>
+      </c>
+      <c r="E34" s="4">
+        <v>48.6</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B35" s="3">
+        <v>-794</v>
+      </c>
+      <c r="C35" s="19">
+        <v>75</v>
+      </c>
+      <c r="D35" s="4">
+        <v>-2025</v>
+      </c>
+      <c r="E35" s="4">
+        <v>48.9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A36" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B36" s="10">
+        <v>-779</v>
+      </c>
+      <c r="C36" s="20">
+        <v>75.400000000000006</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A37" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D37" s="5">
+        <v>-2010</v>
+      </c>
+      <c r="E37" s="5">
+        <v>49.3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A38" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D38" s="4">
+        <v>-2046</v>
+      </c>
+      <c r="E38" s="4">
+        <v>48.4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A39" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D39" s="17">
+        <v>-2010</v>
+      </c>
+      <c r="E39" s="17">
+        <v>49.3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A40" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B35" s="4">
-        <v>-1184</v>
-      </c>
-      <c r="C35" s="4">
-        <v>71.5</v>
-      </c>
-      <c r="D35" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E35" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A38" s="12" t="s">
+      <c r="B40" s="4">
+        <v>-812</v>
+      </c>
+      <c r="C40" s="21">
+        <v>74.400000000000006</v>
+      </c>
+      <c r="D40" s="4">
+        <v>-2067</v>
+      </c>
+      <c r="E40" s="4">
+        <v>47.9</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A43" s="11" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A40" s="1" t="s">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A45" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B45" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C40" s="1"/>
-      <c r="D40" s="1" t="s">
+      <c r="C45" s="1"/>
+      <c r="D45" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A41" s="1"/>
-      <c r="B41" s="2" t="s">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A46" s="1"/>
+      <c r="B46" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C41" s="2" t="s">
+      <c r="C46" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D41" s="2" t="s">
+      <c r="D46" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E41" s="2" t="s">
+      <c r="E46" s="2" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A42" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B42">
-        <v>-5955</v>
-      </c>
-      <c r="C42" s="14">
-        <v>70.900000000000006</v>
-      </c>
-      <c r="D42">
-        <v>-4383</v>
-      </c>
-      <c r="E42">
-        <v>78.900000000000006</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A43" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B43">
-        <v>-5940</v>
-      </c>
-      <c r="C43" s="14">
-        <v>71</v>
-      </c>
-      <c r="D43" s="6">
-        <v>-4308</v>
-      </c>
-      <c r="E43" s="6">
-        <v>79.2</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A44" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B44">
-        <v>-5954</v>
-      </c>
-      <c r="C44" s="14">
-        <v>70.900000000000006</v>
-      </c>
-      <c r="D44">
-        <v>-4382</v>
-      </c>
-      <c r="E44">
-        <v>78.900000000000006</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A45" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B45">
-        <v>-5934</v>
-      </c>
-      <c r="C45" s="14">
-        <v>71</v>
-      </c>
-      <c r="D45">
-        <v>-4337</v>
-      </c>
-      <c r="E45">
-        <v>79.099999999999994</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A46" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B46">
-        <v>-5930</v>
-      </c>
-      <c r="C46" s="14">
-        <v>71</v>
-      </c>
-      <c r="D46">
-        <v>-4343</v>
-      </c>
-      <c r="E46">
-        <v>79</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B47" s="6">
-        <v>-5905</v>
-      </c>
-      <c r="C47" s="15">
-        <v>71.2</v>
+        <v>17</v>
+      </c>
+      <c r="B47">
+        <v>-5955</v>
+      </c>
+      <c r="C47" s="12">
+        <v>70.900000000000006</v>
       </c>
       <c r="D47">
-        <v>-4355</v>
+        <v>-4383</v>
       </c>
       <c r="E47">
-        <v>79</v>
+        <v>78.900000000000006</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B48">
-        <v>-5920</v>
-      </c>
-      <c r="C48" s="14">
-        <v>71.099999999999994</v>
-      </c>
-      <c r="D48">
-        <v>-4387</v>
-      </c>
-      <c r="E48">
-        <v>78.900000000000006</v>
+        <v>-5940</v>
+      </c>
+      <c r="C48" s="12">
+        <v>71</v>
+      </c>
+      <c r="D48" s="6">
+        <v>-4308</v>
+      </c>
+      <c r="E48" s="6">
+        <v>79.2</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" s="2" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="B49">
-        <v>-5983</v>
-      </c>
-      <c r="C49" s="14">
-        <v>70.8</v>
+        <v>-5954</v>
+      </c>
+      <c r="C49" s="12">
+        <v>70.900000000000006</v>
       </c>
       <c r="D49">
-        <v>-4392</v>
+        <v>-4382</v>
       </c>
       <c r="E49">
         <v>78.900000000000006</v>
       </c>
     </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A50" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B50">
+        <v>-5934</v>
+      </c>
+      <c r="C50" s="12">
+        <v>71</v>
+      </c>
+      <c r="D50">
+        <v>-4337</v>
+      </c>
+      <c r="E50">
+        <v>79.099999999999994</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A51" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B51">
+        <v>-5930</v>
+      </c>
+      <c r="C51" s="12">
+        <v>71</v>
+      </c>
+      <c r="D51">
+        <v>-4343</v>
+      </c>
+      <c r="E51">
+        <v>79</v>
+      </c>
+    </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A52" s="16" t="s">
+      <c r="A52" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B52" s="6">
+        <v>-5905</v>
+      </c>
+      <c r="C52" s="13">
+        <v>71.2</v>
+      </c>
+      <c r="D52">
+        <v>-4355</v>
+      </c>
+      <c r="E52">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A53" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B53">
+        <v>-5920</v>
+      </c>
+      <c r="C53" s="12">
+        <v>71.099999999999994</v>
+      </c>
+      <c r="D53">
+        <v>-4387</v>
+      </c>
+      <c r="E53">
+        <v>78.900000000000006</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A54" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B54">
+        <v>-5983</v>
+      </c>
+      <c r="C54" s="12">
+        <v>70.8</v>
+      </c>
+      <c r="D54">
+        <v>-4392</v>
+      </c>
+      <c r="E54">
+        <v>78.900000000000006</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A57" s="14" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A54" s="1" t="s">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A59" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B54" s="1" t="s">
+      <c r="B59" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C54" s="1"/>
-      <c r="D54" s="1" t="s">
+      <c r="C59" s="1"/>
+      <c r="D59" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A55" s="1"/>
-      <c r="B55" s="2" t="s">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A60" s="1"/>
+      <c r="B60" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C55" s="2" t="s">
+      <c r="C60" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D55" s="2" t="s">
+      <c r="D60" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E55" s="2" t="s">
+      <c r="E60" s="2" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A56" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B56">
-        <v>-1643</v>
-      </c>
-      <c r="C56">
-        <v>89.7</v>
-      </c>
-      <c r="D56">
-        <v>-3053</v>
-      </c>
-      <c r="E56">
-        <v>84.3</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A57" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B57">
-        <v>-1640</v>
-      </c>
-      <c r="C57">
-        <v>89.7</v>
-      </c>
-      <c r="D57">
-        <v>-3045</v>
-      </c>
-      <c r="E57">
-        <v>84.3</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A58" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B58">
-        <v>-1642</v>
-      </c>
-      <c r="C58">
-        <v>89.7</v>
-      </c>
-      <c r="D58">
-        <v>-3052</v>
-      </c>
-      <c r="E58">
-        <v>84.3</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A59" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B59">
-        <v>-1643.3</v>
-      </c>
-      <c r="C59">
-        <v>89.7</v>
-      </c>
-      <c r="D59">
-        <v>-3059</v>
-      </c>
-      <c r="E59">
-        <v>84.2</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A60" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B60">
-        <v>-1642</v>
-      </c>
-      <c r="C60">
-        <v>89.7</v>
-      </c>
-      <c r="D60">
-        <v>-3060</v>
-      </c>
-      <c r="E60">
-        <v>84.2</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B61" s="6">
-        <v>-1639</v>
-      </c>
-      <c r="C61" s="6">
+        <v>17</v>
+      </c>
+      <c r="B61">
+        <v>-1643</v>
+      </c>
+      <c r="C61">
         <v>89.7</v>
       </c>
       <c r="D61">
-        <v>-3022</v>
+        <v>-3053</v>
       </c>
       <c r="E61">
-        <v>84.4</v>
+        <v>84.3</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A62" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B62">
-        <v>-1651</v>
+        <v>-1640</v>
       </c>
       <c r="C62">
-        <v>89.6</v>
-      </c>
-      <c r="D62" s="6">
-        <v>-3018</v>
-      </c>
-      <c r="E62" s="6">
-        <v>84.4</v>
+        <v>89.7</v>
+      </c>
+      <c r="D62">
+        <v>-3045</v>
+      </c>
+      <c r="E62">
+        <v>84.3</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63" s="2" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="B63">
         <v>-1642</v>
@@ -1474,177 +1504,262 @@
         <v>89.7</v>
       </c>
       <c r="D63">
+        <v>-3052</v>
+      </c>
+      <c r="E63">
+        <v>84.3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A64" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B64">
+        <v>-1643.3</v>
+      </c>
+      <c r="C64">
+        <v>89.7</v>
+      </c>
+      <c r="D64">
+        <v>-3059</v>
+      </c>
+      <c r="E64">
+        <v>84.2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A65" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B65">
+        <v>-1642</v>
+      </c>
+      <c r="C65">
+        <v>89.7</v>
+      </c>
+      <c r="D65">
+        <v>-3060</v>
+      </c>
+      <c r="E65">
+        <v>84.2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A66" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B66" s="6">
+        <v>-1639</v>
+      </c>
+      <c r="C66" s="6">
+        <v>89.7</v>
+      </c>
+      <c r="D66">
+        <v>-3022</v>
+      </c>
+      <c r="E66">
+        <v>84.4</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A67" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B67">
+        <v>-1651</v>
+      </c>
+      <c r="C67">
+        <v>89.6</v>
+      </c>
+      <c r="D67" s="6">
+        <v>-3018</v>
+      </c>
+      <c r="E67" s="6">
+        <v>84.4</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A68" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B68">
+        <v>-1642</v>
+      </c>
+      <c r="C68">
+        <v>89.7</v>
+      </c>
+      <c r="D68">
         <v>-3071</v>
       </c>
-      <c r="E63">
+      <c r="E68">
         <v>84.2</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A66" s="12" t="s">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A71" s="11" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A68" s="1" t="s">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A73" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B68" s="1" t="s">
+      <c r="B73" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C68" s="1"/>
-      <c r="D68" s="1" t="s">
+      <c r="C73" s="1"/>
+      <c r="D73" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A69" s="1"/>
-      <c r="B69" s="2" t="s">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A74" s="1"/>
+      <c r="B74" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C69" s="2" t="s">
+      <c r="C74" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D69" s="2" t="s">
+      <c r="D74" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E69" s="2" t="s">
+      <c r="E74" s="2" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A70" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B70">
-        <v>-4214</v>
-      </c>
-      <c r="C70">
-        <v>75.5</v>
-      </c>
-      <c r="D70">
-        <v>-2084</v>
-      </c>
-      <c r="E70">
-        <v>84.7</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A71" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B71">
-        <v>-4205</v>
-      </c>
-      <c r="C71">
-        <v>75.5</v>
-      </c>
-      <c r="D71">
-        <v>-2084</v>
-      </c>
-      <c r="E71">
-        <v>84.7</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A72" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B72">
-        <v>-4211</v>
-      </c>
-      <c r="C72">
-        <v>75.5</v>
-      </c>
-      <c r="D72">
-        <v>-2084</v>
-      </c>
-      <c r="E72">
-        <v>84.7</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A73" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B73">
-        <v>-4221</v>
-      </c>
-      <c r="C73">
-        <v>75.400000000000006</v>
-      </c>
-      <c r="D73">
-        <v>-2080</v>
-      </c>
-      <c r="E73">
-        <v>84.7</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A74" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B74">
-        <v>-4226</v>
-      </c>
-      <c r="C74">
-        <v>75.400000000000006</v>
-      </c>
-      <c r="D74">
-        <v>-2079</v>
-      </c>
-      <c r="E74">
-        <v>84.8</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A75" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B75" s="6">
-        <v>-4203</v>
-      </c>
-      <c r="C75" s="6">
+        <v>17</v>
+      </c>
+      <c r="B75">
+        <v>-4214</v>
+      </c>
+      <c r="C75">
         <v>75.5</v>
       </c>
       <c r="D75">
-        <v>-2068</v>
+        <v>-2084</v>
       </c>
       <c r="E75">
-        <v>84.8</v>
+        <v>84.7</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A76" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B76">
-        <v>-4234</v>
+        <v>-4205</v>
       </c>
       <c r="C76">
-        <v>75.3</v>
-      </c>
-      <c r="D76" s="6">
-        <v>-2065</v>
-      </c>
-      <c r="E76" s="6">
-        <v>84.9</v>
+        <v>75.5</v>
+      </c>
+      <c r="D76">
+        <v>-2084</v>
+      </c>
+      <c r="E76">
+        <v>84.7</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A77" s="2" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="B77">
-        <v>-4252</v>
+        <v>-4211</v>
       </c>
       <c r="C77">
-        <v>75.2</v>
+        <v>75.5</v>
       </c>
       <c r="D77">
         <v>-2084</v>
       </c>
       <c r="E77">
+        <v>84.7</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A78" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B78">
+        <v>-4221</v>
+      </c>
+      <c r="C78">
+        <v>75.400000000000006</v>
+      </c>
+      <c r="D78">
+        <v>-2080</v>
+      </c>
+      <c r="E78">
+        <v>84.7</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A79" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B79">
+        <v>-4226</v>
+      </c>
+      <c r="C79">
+        <v>75.400000000000006</v>
+      </c>
+      <c r="D79">
+        <v>-2079</v>
+      </c>
+      <c r="E79">
+        <v>84.8</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A80" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B80" s="6">
+        <v>-4203</v>
+      </c>
+      <c r="C80" s="6">
+        <v>75.5</v>
+      </c>
+      <c r="D80">
+        <v>-2068</v>
+      </c>
+      <c r="E80">
+        <v>84.8</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A81" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B81">
+        <v>-4234</v>
+      </c>
+      <c r="C81">
+        <v>75.3</v>
+      </c>
+      <c r="D81" s="6">
+        <v>-2065</v>
+      </c>
+      <c r="E81" s="6">
+        <v>84.9</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A82" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B82">
+        <v>-4252</v>
+      </c>
+      <c r="C82">
+        <v>75.2</v>
+      </c>
+      <c r="D82">
+        <v>-2084</v>
+      </c>
+      <c r="E82">
         <v>84.7</v>
       </c>
     </row>
@@ -1655,6 +1770,81 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA8B5B52-6AC4-42B2-AC50-DEDF15B4A701}">
+  <dimension ref="D3:E9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="4" max="4" width="16.26953125" customWidth="1"/>
+    <col min="5" max="5" width="13.36328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <v>0.48</v>
+      </c>
+    </row>
+    <row r="5" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5">
+        <v>0.41</v>
+      </c>
+    </row>
+    <row r="6" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="7" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7">
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="8" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8">
+        <v>0.41</v>
+      </c>
+    </row>
+    <row r="9" spans="4:5" x14ac:dyDescent="0.35">
+      <c r="D9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9">
+        <v>0.19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FF19F2C-5071-4FF8-AAF7-6387764C93FA}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
Update with model selection values
</commit_message>
<xml_diff>
--- a/results/hindcast_output/model_selection.xlsx
+++ b/results/hindcast_output/model_selection.xlsx
@@ -8,27 +8,37 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\howar\Documents\Oregon State\ELH_WestCoast\results\hindcast_output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97B80C4D-D1A7-49AF-B7E8-A54B57EB86D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1D3CDE2-A4F3-4EDE-B6F8-704D72F6BE5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Models" sheetId="1" r:id="rId1"/>
     <sheet name="Statistics" sheetId="2" r:id="rId2"/>
     <sheet name="Schoener's D" sheetId="4" r:id="rId3"/>
-    <sheet name="Cross Validation" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="51">
   <si>
     <t>Species</t>
   </si>
@@ -178,6 +188,9 @@
   </si>
   <si>
     <t>2080-2010</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -305,8 +318,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -318,13 +329,17 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -613,8 +628,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -642,7 +657,7 @@
       <c r="B2" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="17" t="s">
         <v>43</v>
       </c>
       <c r="E2" t="s">
@@ -653,10 +668,10 @@
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="16" t="s">
         <v>40</v>
       </c>
       <c r="E3" t="s">
@@ -667,10 +682,10 @@
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="19" t="s">
         <v>44</v>
       </c>
       <c r="E4" t="s">
@@ -695,7 +710,7 @@
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="12" t="s">
         <v>14</v>
       </c>
       <c r="C6" s="7" t="s">
@@ -709,10 +724,10 @@
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="C7" s="21" t="s">
+      <c r="C7" s="18" t="s">
         <v>45</v>
       </c>
       <c r="E7" t="s">
@@ -763,8 +778,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{494A45B2-305D-490A-9F7F-E122BE2F71EC}">
   <dimension ref="A1:E82"/>
   <sheetViews>
-    <sheetView topLeftCell="A71" workbookViewId="0">
-      <selection activeCell="B75" sqref="B75:E82"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I78" sqref="I78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -828,10 +843,10 @@
       <c r="A6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="18">
+      <c r="B6" s="4">
         <v>-7637</v>
       </c>
-      <c r="C6" s="18">
+      <c r="C6" s="4">
         <v>64.8</v>
       </c>
       <c r="D6" s="4">
@@ -979,73 +994,137 @@
       <c r="A19" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
+      <c r="B19" s="3">
+        <v>-987</v>
+      </c>
+      <c r="C19" s="3">
+        <v>74.2</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="9"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
+      <c r="B20" s="21">
+        <v>-987</v>
+      </c>
+      <c r="C20" s="21">
+        <v>74.2</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
+      <c r="B21" s="3">
+        <v>-986</v>
+      </c>
+      <c r="C21" s="3">
+        <v>74.2</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
+      <c r="B22" s="3">
+        <v>-982</v>
+      </c>
+      <c r="C22" s="3">
+        <v>74.400000000000006</v>
+      </c>
+      <c r="D22" s="3">
+        <v>-1410</v>
+      </c>
+      <c r="E22" s="3">
+        <v>67.8</v>
+      </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
+      <c r="B23" s="9">
+        <v>-981</v>
+      </c>
+      <c r="C23" s="9">
+        <v>74.400000000000006</v>
+      </c>
+      <c r="D23" s="9">
+        <v>-1408</v>
+      </c>
+      <c r="E23" s="9">
+        <v>67.8</v>
+      </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
+      <c r="B24" s="3">
+        <v>-987</v>
+      </c>
+      <c r="C24" s="3">
+        <v>74.2</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
+      <c r="B25" s="3">
+        <v>-983</v>
+      </c>
+      <c r="C25" s="3">
+        <v>74.3</v>
+      </c>
+      <c r="D25" s="3">
+        <v>-1419</v>
+      </c>
+      <c r="E25" s="3">
+        <v>67.599999999999994</v>
+      </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
+      <c r="B26" s="3">
+        <v>-988</v>
+      </c>
+      <c r="C26" s="3">
+        <v>74.2</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="2"/>
@@ -1090,73 +1169,137 @@
       <c r="A33" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B33" s="3"/>
-      <c r="C33" s="15"/>
-      <c r="D33" s="4"/>
-      <c r="E33" s="4"/>
+      <c r="B33" s="3">
+        <v>-880</v>
+      </c>
+      <c r="C33" s="13">
+        <v>76.099999999999994</v>
+      </c>
+      <c r="D33" s="4">
+        <v>-2491</v>
+      </c>
+      <c r="E33" s="4">
+        <v>46.7</v>
+      </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B34" s="3"/>
-      <c r="C34" s="15"/>
-      <c r="D34" s="4"/>
-      <c r="E34" s="4"/>
+      <c r="B34" s="3">
+        <v>-896</v>
+      </c>
+      <c r="C34" s="13">
+        <v>75.7</v>
+      </c>
+      <c r="D34" s="4">
+        <v>-2512</v>
+      </c>
+      <c r="E34" s="4">
+        <v>46.2</v>
+      </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B35" s="3"/>
-      <c r="C35" s="15"/>
-      <c r="D35" s="4"/>
-      <c r="E35" s="4"/>
+      <c r="B35" s="3">
+        <v>-878</v>
+      </c>
+      <c r="C35" s="13">
+        <v>76.2</v>
+      </c>
+      <c r="D35" s="4">
+        <v>-2487</v>
+      </c>
+      <c r="E35" s="4">
+        <v>46.8</v>
+      </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B36" s="9"/>
-      <c r="C36" s="16"/>
-      <c r="D36" s="4"/>
-      <c r="E36" s="4"/>
+      <c r="B36" s="9">
+        <v>-876</v>
+      </c>
+      <c r="C36" s="14">
+        <v>76.3</v>
+      </c>
+      <c r="D36" s="5">
+        <v>-2462</v>
+      </c>
+      <c r="E36" s="5">
+        <v>47.3</v>
+      </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B37" s="3"/>
-      <c r="C37" s="3"/>
-      <c r="D37" s="5"/>
-      <c r="E37" s="5"/>
+      <c r="B37" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D37" s="4">
+        <v>-2466</v>
+      </c>
+      <c r="E37" s="4">
+        <v>47.2</v>
+      </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B38" s="3"/>
-      <c r="C38" s="3"/>
-      <c r="D38" s="4"/>
-      <c r="E38" s="4"/>
+      <c r="B38" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B39" s="3"/>
-      <c r="C39" s="3"/>
-      <c r="D39" s="4"/>
-      <c r="E39" s="4"/>
+      <c r="B39" s="3">
+        <v>-896</v>
+      </c>
+      <c r="C39" s="3">
+        <v>75.7</v>
+      </c>
+      <c r="D39" s="4">
+        <v>-2474</v>
+      </c>
+      <c r="E39" s="4">
+        <v>47</v>
+      </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B40" s="4"/>
-      <c r="C40" s="17"/>
-      <c r="D40" s="4"/>
-      <c r="E40" s="4"/>
+      <c r="B40" s="4">
+        <v>-899</v>
+      </c>
+      <c r="C40" s="15">
+        <v>75.7</v>
+      </c>
+      <c r="D40" s="4">
+        <v>-2531</v>
+      </c>
+      <c r="E40" s="4">
+        <v>45.8</v>
+      </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" s="10" t="s">
@@ -1194,55 +1337,140 @@
       <c r="A47" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C47" s="11"/>
+      <c r="B47" s="4">
+        <v>-5952</v>
+      </c>
+      <c r="C47" s="15">
+        <v>70.900000000000006</v>
+      </c>
+      <c r="D47" s="4">
+        <v>-4386</v>
+      </c>
+      <c r="E47" s="4">
+        <v>78.900000000000006</v>
+      </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C48" s="11"/>
-      <c r="D48" s="6"/>
-      <c r="E48" s="6"/>
+      <c r="B48" s="4">
+        <v>-5956</v>
+      </c>
+      <c r="C48" s="15">
+        <v>70.900000000000006</v>
+      </c>
+      <c r="D48" s="5">
+        <v>-4333</v>
+      </c>
+      <c r="E48" s="5">
+        <v>79.099999999999994</v>
+      </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C49" s="11"/>
+      <c r="B49" s="4">
+        <v>-5952</v>
+      </c>
+      <c r="C49" s="15">
+        <v>70.900000000000006</v>
+      </c>
+      <c r="D49" s="4">
+        <v>-4384</v>
+      </c>
+      <c r="E49" s="4">
+        <v>78.900000000000006</v>
+      </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C50" s="11"/>
+      <c r="B50" s="4">
+        <v>-5930</v>
+      </c>
+      <c r="C50" s="15">
+        <v>71</v>
+      </c>
+      <c r="D50" s="4">
+        <v>-4340</v>
+      </c>
+      <c r="E50" s="4">
+        <v>79.099999999999994</v>
+      </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C51" s="11"/>
+      <c r="B51" s="4">
+        <v>-5925</v>
+      </c>
+      <c r="C51" s="15">
+        <v>71.099999999999994</v>
+      </c>
+      <c r="D51" s="4">
+        <v>-4346</v>
+      </c>
+      <c r="E51" s="4">
+        <v>79.099999999999994</v>
+      </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B52" s="6"/>
-      <c r="C52" s="12"/>
+      <c r="B52" s="5">
+        <v>-5908</v>
+      </c>
+      <c r="C52" s="22">
+        <v>71.2</v>
+      </c>
+      <c r="D52" s="4">
+        <v>-4360</v>
+      </c>
+      <c r="E52" s="4">
+        <v>79</v>
+      </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C53" s="11"/>
+      <c r="B53" s="4">
+        <v>-5919</v>
+      </c>
+      <c r="C53" s="15">
+        <v>71.099999999999994</v>
+      </c>
+      <c r="D53" s="4">
+        <v>-4390</v>
+      </c>
+      <c r="E53" s="4">
+        <v>78.900000000000006</v>
+      </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C54" s="11"/>
+      <c r="B54" s="4">
+        <v>-5891</v>
+      </c>
+      <c r="C54" s="15">
+        <v>70.8</v>
+      </c>
+      <c r="D54" s="4">
+        <v>-4384</v>
+      </c>
+      <c r="E54" s="4">
+        <v>78.8</v>
+      </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A57" s="13" t="s">
+      <c r="A57" s="11" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1277,44 +1505,136 @@
       <c r="A61" s="2" t="s">
         <v>17</v>
       </c>
+      <c r="B61" s="4">
+        <v>-1637</v>
+      </c>
+      <c r="C61" s="4">
+        <v>89.7</v>
+      </c>
+      <c r="D61" s="4">
+        <v>-3036</v>
+      </c>
+      <c r="E61" s="4">
+        <v>84.4</v>
+      </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A62" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="B62" s="4">
+        <v>-1649</v>
+      </c>
+      <c r="C62" s="4">
+        <v>89.6</v>
+      </c>
+      <c r="D62" s="4">
+        <v>-3055</v>
+      </c>
+      <c r="E62" s="4">
+        <v>84.3</v>
+      </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="B63" s="5">
+        <v>-1636</v>
+      </c>
+      <c r="C63" s="5">
+        <v>89.7</v>
+      </c>
+      <c r="D63" s="4">
+        <v>-3034</v>
+      </c>
+      <c r="E63" s="4">
+        <v>84.4</v>
+      </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A64" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="B64" s="4">
+        <v>-1645</v>
+      </c>
+      <c r="C64" s="4">
+        <v>89.7</v>
+      </c>
+      <c r="D64" s="4">
+        <v>-3056</v>
+      </c>
+      <c r="E64" s="4">
+        <v>84.3</v>
+      </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="B65" s="4">
+        <v>-1644</v>
+      </c>
+      <c r="C65" s="4">
+        <v>89.7</v>
+      </c>
+      <c r="D65" s="4">
+        <v>-3057</v>
+      </c>
+      <c r="E65" s="4">
+        <v>84.2</v>
+      </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A66" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B66" s="6"/>
-      <c r="C66" s="6"/>
+      <c r="B66" s="4">
+        <v>-1641</v>
+      </c>
+      <c r="C66" s="4">
+        <v>89.7</v>
+      </c>
+      <c r="D66" s="4">
+        <v>-3015</v>
+      </c>
+      <c r="E66" s="4">
+        <v>84.5</v>
+      </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A67" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D67" s="6"/>
-      <c r="E67" s="6"/>
+      <c r="B67" s="4">
+        <v>-1654</v>
+      </c>
+      <c r="C67" s="4">
+        <v>89.6</v>
+      </c>
+      <c r="D67" s="5">
+        <v>-3014</v>
+      </c>
+      <c r="E67" s="5">
+        <v>84.5</v>
+      </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A68" s="2" t="s">
         <v>22</v>
+      </c>
+      <c r="B68" s="4">
+        <v>-1655</v>
+      </c>
+      <c r="C68" s="4">
+        <v>89.6</v>
+      </c>
+      <c r="D68" s="4">
+        <v>-3066</v>
+      </c>
+      <c r="E68" s="4">
+        <v>84.2</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.35">
@@ -1353,44 +1673,136 @@
       <c r="A75" s="2" t="s">
         <v>17</v>
       </c>
+      <c r="B75" s="4">
+        <v>-4214</v>
+      </c>
+      <c r="C75" s="4">
+        <v>75.5</v>
+      </c>
+      <c r="D75" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E75" s="4" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A76" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="B76" s="4">
+        <v>-4246</v>
+      </c>
+      <c r="C76" s="4">
+        <v>75.3</v>
+      </c>
+      <c r="D76" s="4">
+        <v>-2082</v>
+      </c>
+      <c r="E76" s="4">
+        <v>84.7</v>
+      </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A77" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="B77" s="4">
+        <v>-4211</v>
+      </c>
+      <c r="C77" s="4">
+        <v>75.5</v>
+      </c>
+      <c r="D77" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E77" s="4" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A78" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="B78" s="4">
+        <v>-4220</v>
+      </c>
+      <c r="C78" s="4">
+        <v>75.400000000000006</v>
+      </c>
+      <c r="D78" s="4">
+        <v>-2080</v>
+      </c>
+      <c r="E78" s="4">
+        <v>84.7</v>
+      </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A79" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="B79" s="4">
+        <v>-4225</v>
+      </c>
+      <c r="C79" s="4">
+        <v>75.400000000000006</v>
+      </c>
+      <c r="D79" s="4">
+        <v>-2079</v>
+      </c>
+      <c r="E79" s="4">
+        <v>84.8</v>
+      </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A80" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B80" s="6"/>
-      <c r="C80" s="6"/>
+      <c r="B80" s="5">
+        <v>-4202</v>
+      </c>
+      <c r="C80" s="5">
+        <v>75.5</v>
+      </c>
+      <c r="D80" s="4">
+        <v>-2067</v>
+      </c>
+      <c r="E80" s="4">
+        <v>84.8</v>
+      </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A81" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D81" s="6"/>
-      <c r="E81" s="6"/>
+      <c r="B81" s="4">
+        <v>-4234</v>
+      </c>
+      <c r="C81" s="4">
+        <v>75.3</v>
+      </c>
+      <c r="D81" s="5">
+        <v>-2064</v>
+      </c>
+      <c r="E81" s="5">
+        <v>84.9</v>
+      </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A82" s="2" t="s">
         <v>22</v>
+      </c>
+      <c r="B82" s="4">
+        <v>-4252</v>
+      </c>
+      <c r="C82" s="4">
+        <v>75.2</v>
+      </c>
+      <c r="D82" s="4">
+        <v>-2088</v>
+      </c>
+      <c r="E82" s="4">
+        <v>84.7</v>
       </c>
     </row>
   </sheetData>
@@ -1403,8 +1815,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA8B5B52-6AC4-42B2-AC50-DEDF15B4A701}">
   <dimension ref="D1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1448,8 +1860,17 @@
       <c r="D4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E4">
-        <v>0.62</v>
+      <c r="E4" s="20">
+        <v>0.6</v>
+      </c>
+      <c r="F4">
+        <v>0.46</v>
+      </c>
+      <c r="G4">
+        <v>0.45</v>
+      </c>
+      <c r="H4">
+        <v>0.45</v>
       </c>
     </row>
     <row r="5" spans="4:8" x14ac:dyDescent="0.35">
@@ -1457,7 +1878,16 @@
         <v>4</v>
       </c>
       <c r="E5">
-        <v>0.36</v>
+        <v>0.76</v>
+      </c>
+      <c r="F5">
+        <v>0.68</v>
+      </c>
+      <c r="G5">
+        <v>0.66</v>
+      </c>
+      <c r="H5">
+        <v>0.65</v>
       </c>
     </row>
     <row r="6" spans="4:8" x14ac:dyDescent="0.35">
@@ -1465,7 +1895,16 @@
         <v>5</v>
       </c>
       <c r="E6">
-        <v>0.57999999999999996</v>
+        <v>0.51</v>
+      </c>
+      <c r="F6">
+        <v>0.48</v>
+      </c>
+      <c r="G6" s="20">
+        <v>0.5</v>
+      </c>
+      <c r="H6" s="20">
+        <v>0.5</v>
       </c>
     </row>
     <row r="7" spans="4:8" x14ac:dyDescent="0.35">
@@ -1473,7 +1912,16 @@
         <v>6</v>
       </c>
       <c r="E7">
-        <v>0.52</v>
+        <v>0.64</v>
+      </c>
+      <c r="F7">
+        <v>0.63</v>
+      </c>
+      <c r="G7">
+        <v>0.63</v>
+      </c>
+      <c r="H7">
+        <v>0.63</v>
       </c>
     </row>
     <row r="8" spans="4:8" x14ac:dyDescent="0.35">
@@ -1481,7 +1929,16 @@
         <v>7</v>
       </c>
       <c r="E8">
-        <v>0.28000000000000003</v>
+        <v>0.52</v>
+      </c>
+      <c r="F8">
+        <v>0.54</v>
+      </c>
+      <c r="G8">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="H8">
+        <v>0.54</v>
       </c>
     </row>
     <row r="9" spans="4:8" x14ac:dyDescent="0.35">
@@ -1489,22 +1946,19 @@
         <v>8</v>
       </c>
       <c r="E9">
-        <v>0.26</v>
+        <v>0.64</v>
+      </c>
+      <c r="F9">
+        <v>0.63</v>
+      </c>
+      <c r="G9">
+        <v>0.66</v>
+      </c>
+      <c r="H9">
+        <v>0.64</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FF19F2C-5071-4FF8-AAF7-6387764C93FA}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Update using custom mesh function, new scripts for last species
</commit_message>
<xml_diff>
--- a/results/hindcast_output/model_selection.xlsx
+++ b/results/hindcast_output/model_selection.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20415"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rebecca.howard\Work\Projects\ELH_WestCoast\results\hindcast_output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B44EC62F-E40B-4214-AB1A-33B002E7DF0F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40D7EA01-3540-4552-91A9-E3490A99327E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12375" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="52">
   <si>
     <t>Species</t>
   </si>
@@ -68,9 +68,6 @@
     <t>u_vint_50m: u-eastward vertically integrated from 0-50m and averaged from coast to 50 km offshore</t>
   </si>
   <si>
-    <t>spice</t>
-  </si>
-  <si>
     <t>vmax_cu</t>
   </si>
   <si>
@@ -107,9 +104,6 @@
     <t>Log-likelihood</t>
   </si>
   <si>
-    <t>iso26</t>
-  </si>
-  <si>
     <t>vgeo: surface geostrophic v-component avg from coast to 50km</t>
   </si>
   <si>
@@ -155,12 +149,6 @@
     <t>* significant</t>
   </si>
   <si>
-    <t>iso26*</t>
-  </si>
-  <si>
-    <t>uvint 50m*</t>
-  </si>
-  <si>
     <t>spice*</t>
   </si>
   <si>
@@ -182,7 +170,19 @@
     <t>ios26</t>
   </si>
   <si>
-    <t>base*</t>
+    <t>uvint 100m*</t>
+  </si>
+  <si>
+    <t>uvint 100m</t>
+  </si>
+  <si>
+    <t>base: no variable</t>
+  </si>
+  <si>
+    <t>u_vint_50m</t>
+  </si>
+  <si>
+    <t>u_vint_100m</t>
   </si>
 </sst>
 </file>
@@ -581,7 +581,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -601,6 +601,9 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -610,7 +613,7 @@
         <v>50</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>42</v>
+        <v>13</v>
       </c>
       <c r="E2" t="s">
         <v>9</v>
@@ -624,7 +627,7 @@
         <v>51</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E3" t="s">
         <v>10</v>
@@ -635,10 +638,10 @@
         <v>5</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="C4" s="14" t="s">
-        <v>43</v>
+        <v>47</v>
+      </c>
+      <c r="C4" t="s">
+        <v>40</v>
       </c>
       <c r="E4" t="s">
         <v>11</v>
@@ -649,10 +652,10 @@
         <v>6</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="E5" t="s">
         <v>12</v>
@@ -663,13 +666,13 @@
         <v>7</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -677,48 +680,48 @@
         <v>8</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="E7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -745,12 +748,12 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>1</v>
@@ -763,21 +766,21 @@
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>25</v>
-      </c>
       <c r="E4" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5" s="4">
         <v>-7643</v>
@@ -794,7 +797,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B6" s="4">
         <v>-7637</v>
@@ -811,7 +814,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7" s="4">
         <v>-7647</v>
@@ -828,7 +831,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8" s="4">
         <v>-7640</v>
@@ -845,7 +848,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B9" s="4">
         <v>-7642</v>
@@ -862,7 +865,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B10" s="5">
         <v>-7613</v>
@@ -879,7 +882,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B11" s="4">
         <v>-7642</v>
@@ -896,7 +899,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B12" s="4">
         <v>-7666</v>
@@ -913,12 +916,12 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>1</v>
@@ -931,21 +934,21 @@
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C18" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D18" s="2" t="s">
-        <v>25</v>
-      </c>
       <c r="E18" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B19" s="3">
         <v>-987</v>
@@ -954,15 +957,15 @@
         <v>74.2</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B20" s="3">
         <v>-987</v>
@@ -971,15 +974,15 @@
         <v>74.2</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B21" s="3">
         <v>-986</v>
@@ -988,15 +991,15 @@
         <v>74.2</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B22" s="3">
         <v>-982</v>
@@ -1013,7 +1016,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B23" s="6">
         <v>-981</v>
@@ -1030,7 +1033,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B24" s="3">
         <v>-987</v>
@@ -1039,15 +1042,15 @@
         <v>74.2</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B25" s="3">
         <v>-983</v>
@@ -1064,7 +1067,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B26" s="3">
         <v>-988</v>
@@ -1073,10 +1076,10 @@
         <v>74.2</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -1088,12 +1091,12 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>1</v>
@@ -1106,21 +1109,21 @@
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C32" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D32" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D32" s="2" t="s">
-        <v>25</v>
-      </c>
       <c r="E32" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B33" s="3">
         <v>-880</v>
@@ -1137,7 +1140,7 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B34" s="3">
         <v>-896</v>
@@ -1154,7 +1157,7 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B35" s="3">
         <v>-878</v>
@@ -1171,7 +1174,7 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B36" s="6">
         <v>-876</v>
@@ -1188,13 +1191,13 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D37" s="4">
         <v>-2466</v>
@@ -1205,24 +1208,24 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B39" s="3">
         <v>-896</v>
@@ -1239,7 +1242,7 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B40" s="4">
         <v>-899</v>
@@ -1256,12 +1259,12 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>1</v>
@@ -1274,21 +1277,21 @@
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C46" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D46" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D46" s="2" t="s">
-        <v>25</v>
-      </c>
       <c r="E46" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B47" s="4">
         <v>-5952</v>
@@ -1305,7 +1308,7 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B48" s="4">
         <v>-5956</v>
@@ -1322,7 +1325,7 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B49" s="4">
         <v>-5952</v>
@@ -1339,7 +1342,7 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B50" s="4">
         <v>-5930</v>
@@ -1356,7 +1359,7 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B51" s="4">
         <v>-5925</v>
@@ -1373,7 +1376,7 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B52" s="5">
         <v>-5908</v>
@@ -1390,7 +1393,7 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B53" s="4">
         <v>-5919</v>
@@ -1407,7 +1410,7 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B54" s="4">
         <v>-5891</v>
@@ -1424,12 +1427,12 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>1</v>
@@ -1442,21 +1445,21 @@
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C60" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D60" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D60" s="2" t="s">
-        <v>25</v>
-      </c>
       <c r="E60" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B61" s="4">
         <v>-1637</v>
@@ -1473,7 +1476,7 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B62" s="4">
         <v>-1649</v>
@@ -1490,7 +1493,7 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B63" s="5">
         <v>-1636</v>
@@ -1507,7 +1510,7 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B64" s="4">
         <v>-1645</v>
@@ -1524,7 +1527,7 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B65" s="4">
         <v>-1644</v>
@@ -1541,7 +1544,7 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B66" s="4">
         <v>-1641</v>
@@ -1558,7 +1561,7 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B67" s="4">
         <v>-1654</v>
@@ -1575,7 +1578,7 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B68" s="4">
         <v>-1655</v>
@@ -1592,12 +1595,12 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>1</v>
@@ -1610,21 +1613,21 @@
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
       <c r="B74" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C74" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D74" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D74" s="2" t="s">
-        <v>25</v>
-      </c>
       <c r="E74" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B75" s="4">
         <v>-4214</v>
@@ -1633,15 +1636,15 @@
         <v>75.5</v>
       </c>
       <c r="D75" s="4" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E75" s="4" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B76" s="4">
         <v>-4246</v>
@@ -1658,7 +1661,7 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B77" s="4">
         <v>-4211</v>
@@ -1667,15 +1670,15 @@
         <v>75.5</v>
       </c>
       <c r="D77" s="4" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E77" s="4" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B78" s="4">
         <v>-4220</v>
@@ -1692,7 +1695,7 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B79" s="4">
         <v>-4225</v>
@@ -1709,7 +1712,7 @@
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B80" s="5">
         <v>-4202</v>
@@ -1726,7 +1729,7 @@
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B81" s="4">
         <v>-4234</v>
@@ -1743,7 +1746,7 @@
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B82" s="4">
         <v>-4252</v>
@@ -1783,7 +1786,7 @@
   <sheetData>
     <row r="1" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D1" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="4:8" x14ac:dyDescent="0.25">
@@ -1797,16 +1800,16 @@
         <v>0</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="4:8" x14ac:dyDescent="0.25">

</xml_diff>